<commit_message>
excel sheet updated with negative test cases
</commit_message>
<xml_diff>
--- a/Expense Tracker.xlsx
+++ b/Expense Tracker.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Positive Test Cases" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="123">
   <si>
     <t xml:space="preserve">TestCase Id</t>
   </si>
@@ -315,7 +315,88 @@
     <t xml:space="preserve">Expected </t>
   </si>
   <si>
-    <t xml:space="preserve">Can be automated</t>
+    <t xml:space="preserve">Verify if the user is able to add 0 as a amount in expense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should not be able to add 0 amount in expense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User is able to add 0 amount in expense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amount - 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.Click on amount field and enter amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.Click on add</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.Verify if the 0 amount is getting added and appearing in all entries screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify if the currency displayed in the amount field in expense screen is same as the actual currency updated in settings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Currency in the amount field should be same as updated currency in settings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updated currency is USD and currency is displayed in euro in expense screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.Fetch currency from the amount field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.Click on profile button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.Fetch currency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.Compare currency from settings  and currency in amount field in the expense screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify if the user is able to add account name of any length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AccountName – UserAccountNameLengthTesting123456789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should not be able to add account of length more than 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user is able to add account with length more than 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.Fetch Added account name and fetch the length of that</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.Verify if the length of account name is more than 20 or not</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify if the user is able to add expense after adding wrong date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should not be able to add expense with wrong date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User is able to add expense with wrong date like 6 digits in year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category – Health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description – Medicine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date – 06/03/202020, 21:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.Fetch Category from the all entries that verifies that it is getting added</t>
   </si>
   <si>
     <t xml:space="preserve">Verfiy if it is again going to the profile page on clicking browser back button after logout</t>
@@ -327,52 +408,10 @@
     <t xml:space="preserve">User is able to see profile even after logout</t>
   </si>
   <si>
-    <t xml:space="preserve">Fail(Manually Tested)</t>
-  </si>
-  <si>
     <t xml:space="preserve">7.Click on logout button</t>
   </si>
   <si>
     <t xml:space="preserve">8.Click on browser back button</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verify if the currency displayed in the amount field in expense screen is same as the actual currency updated in settings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Currency in the amount field should be same as updated currency in settings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Updated currency is USD and currency is displayed in euro in expense screen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.Fetch currency from the amount field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.Click on profile button</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.Fetch currency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.Compare currency from settings  and currency in amount field in the expense screen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verify if the user is able to add 0 as a amount in expense</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User should not be able to add 0 amount in expense</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User is able to add 0 amount in expense</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amount - 0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.Click on amount field and enter amount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.Click on add</t>
   </si>
 </sst>
 </file>
@@ -477,7 +516,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -506,7 +545,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -529,8 +576,8 @@
   </sheetPr>
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C62" activeCellId="0" sqref="C62"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B17" activeCellId="1" sqref="F1:G1 B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -539,7 +586,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="55.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="46.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="46.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="54.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.63"/>
@@ -1322,7 +1369,6 @@
       <c r="F56" s="4"/>
       <c r="G56" s="4"/>
     </row>
-    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1358,20 +1404,20 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="49.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="37.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="40.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="37.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="40.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="14.43"/>
   </cols>
   <sheetData>
@@ -1397,204 +1443,353 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>90</v>
-      </c>
+      <c r="H1" s="2"/>
       <c r="I1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="5" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="5" t="s">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="8" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="n">
         <v>2</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C10" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="4" t="s">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="4" t="s">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="4" t="s">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="n">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="B19" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D26" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="4" t="s">
+      <c r="E26" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D27" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="4" t="s">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C28" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="4" t="s">
+      <c r="D28" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="7" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="4" t="s">
+      <c r="D29" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="7" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="7" t="s">
-        <v>109</v>
+      <c r="D30" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C39" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C40" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C41" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C42" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C43" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C44" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C45" s="5" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>